<commit_message>
complete usergroup permission update
</commit_message>
<xml_diff>
--- a/zabbix_usergroup.xlsx
+++ b/zabbix_usergroup.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7">
   <si>
     <t>用户组（group name）</t>
   </si>
@@ -34,9 +34,6 @@
     <t>wangjinle-hostgroup</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t>Zabbix servers</t>
   </si>
   <si>
@@ -48,10 +45,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -72,37 +69,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -131,6 +97,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -138,32 +135,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -191,19 +175,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,6 +226,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -253,25 +274,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -319,12 +364,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -344,48 +383,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,50 +460,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -535,6 +488,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -543,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -555,142 +552,145 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1043,7 +1043,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1064,7 +1064,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1075,19 +1075,18 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3">
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>2</v>

</xml_diff>